<commit_message>
Working through notebook 3
</commit_message>
<xml_diff>
--- a/excel/britlit.xlsx
+++ b/excel/britlit.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18067"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rache\Documents\Camtasia Studio\NumLinAlg\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\willk\OneDrive\Documents\git\fastai-numerical-linear-algebra\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2010" yWindow="0" windowWidth="12735" windowHeight="11415"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="11040" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="6" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="126">
   <si>
     <t>Topic 1</t>
   </si>
@@ -1301,40 +1301,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="103.5703125" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="103.5546875" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="37.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" ht="36" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" ht="54" x14ac:dyDescent="0.35">
       <c r="A3" s="11" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" s="11"/>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>125</v>
       </c>
@@ -1349,19 +1349,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BM28"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="R1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AF12" sqref="AF12"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A2" sqref="A2:A28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.5703125" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" customWidth="1"/>
-    <col min="46" max="46" width="11.7109375" customWidth="1"/>
+    <col min="1" max="1" width="32.5546875" customWidth="1"/>
+    <col min="6" max="6" width="11.88671875" customWidth="1"/>
+    <col min="46" max="46" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:65" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:65" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B1" s="8" t="s">
         <v>40</v>
       </c>
@@ -1555,7 +1555,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:65" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:65" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
@@ -1752,7 +1752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:65" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:65" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>14</v>
       </c>
@@ -1949,7 +1949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:65" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:65" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>15</v>
       </c>
@@ -2146,7 +2146,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:65" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:65" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>16</v>
       </c>
@@ -2343,7 +2343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:65" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:65" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>17</v>
       </c>
@@ -2540,7 +2540,7 @@
         <v>0.17713970971151999</v>
       </c>
     </row>
-    <row r="7" spans="1:65" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:65" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>18</v>
       </c>
@@ -2737,7 +2737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:65" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:65" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>19</v>
       </c>
@@ -2934,7 +2934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:65" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:65" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>20</v>
       </c>
@@ -3131,7 +3131,7 @@
         <v>4.6961748415000001E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:65" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:65" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>21</v>
       </c>
@@ -3328,7 +3328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:65" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:65" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>22</v>
       </c>
@@ -3525,7 +3525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:65" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:65" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>23</v>
       </c>
@@ -3722,7 +3722,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:65" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:65" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>24</v>
       </c>
@@ -3919,7 +3919,7 @@
         <v>3.5668663302000002E-4</v>
       </c>
     </row>
-    <row r="14" spans="1:65" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:65" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>25</v>
       </c>
@@ -4116,7 +4116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:65" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:65" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>26</v>
       </c>
@@ -4313,7 +4313,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:65" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:65" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>27</v>
       </c>
@@ -4510,7 +4510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:65" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:65" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>28</v>
       </c>
@@ -4707,7 +4707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:65" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:65" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>29</v>
       </c>
@@ -4904,7 +4904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:65" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:65" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>30</v>
       </c>
@@ -5101,7 +5101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:65" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:65" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
         <v>31</v>
       </c>
@@ -5298,7 +5298,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:65" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:65" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
         <v>32</v>
       </c>
@@ -5495,7 +5495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:65" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:65" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
         <v>33</v>
       </c>
@@ -5692,7 +5692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:65" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:65" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
         <v>34</v>
       </c>
@@ -5889,7 +5889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:65" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:65" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
         <v>35</v>
       </c>
@@ -6086,7 +6086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:65" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:65" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
         <v>36</v>
       </c>
@@ -6283,7 +6283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:65" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:65" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
         <v>37</v>
       </c>
@@ -6480,7 +6480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:65" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:65" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
         <v>38</v>
       </c>
@@ -6677,7 +6677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:65" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:65" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="7" t="s">
         <v>12</v>
       </c>
@@ -6881,32 +6881,32 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BY42"/>
+  <dimension ref="A1:BY51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+    <sheetView topLeftCell="M4" workbookViewId="0">
+      <selection activeCell="AB27" sqref="AB27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.42578125" style="1" customWidth="1"/>
-    <col min="2" max="3" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" style="1" customWidth="1"/>
-    <col min="5" max="11" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="9.140625" style="1"/>
-    <col min="14" max="23" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.140625" style="1"/>
+    <col min="1" max="1" width="34.44140625" style="1" customWidth="1"/>
+    <col min="2" max="3" width="17.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5546875" style="1" customWidth="1"/>
+    <col min="5" max="11" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="9.109375" style="1"/>
+    <col min="14" max="23" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.109375" style="1"/>
     <col min="25" max="25" width="12" style="1" customWidth="1"/>
-    <col min="26" max="26" width="10.85546875" style="1" customWidth="1"/>
-    <col min="27" max="27" width="11.7109375" style="1" customWidth="1"/>
-    <col min="28" max="28" width="12.140625" style="1" customWidth="1"/>
-    <col min="29" max="29" width="11.5703125" style="1" customWidth="1"/>
+    <col min="26" max="26" width="10.88671875" style="1" customWidth="1"/>
+    <col min="27" max="27" width="11.6640625" style="1" customWidth="1"/>
+    <col min="28" max="28" width="12.109375" style="1" customWidth="1"/>
+    <col min="29" max="29" width="11.5546875" style="1" customWidth="1"/>
     <col min="30" max="30" width="12" style="1" customWidth="1"/>
-    <col min="31" max="77" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="78" max="16384" width="9.140625" style="1"/>
+    <col min="31" max="77" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="78" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:77" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>104</v>
       </c>
@@ -7133,7 +7133,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="2" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:77" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>13</v>
       </c>
@@ -7360,7 +7360,7 @@
         <v>3.6630699193830003E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:77" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>14</v>
       </c>
@@ -7587,7 +7587,7 @@
         <v>-8.6857441839990002E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:77" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
         <v>15</v>
       </c>
@@ -7814,7 +7814,7 @@
         <v>-4.4451027151169997E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:77" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
         <v>16</v>
       </c>
@@ -8041,7 +8041,7 @@
         <v>0.15569753496552999</v>
       </c>
     </row>
-    <row r="6" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:77" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
         <v>17</v>
       </c>
@@ -8268,7 +8268,7 @@
         <v>-2.6685795412099999E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:77" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
         <v>18</v>
       </c>
@@ -8495,7 +8495,7 @@
         <v>4.7469727824000003E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:77" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
         <v>19</v>
       </c>
@@ -8722,7 +8722,7 @@
         <v>0.12945000089393999</v>
       </c>
     </row>
-    <row r="9" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:77" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="s">
         <v>20</v>
       </c>
@@ -8949,7 +8949,7 @@
         <v>-0.10333637705642</v>
       </c>
     </row>
-    <row r="10" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:77" x14ac:dyDescent="0.35">
       <c r="A10" s="6" t="s">
         <v>21</v>
       </c>
@@ -9176,7 +9176,7 @@
         <v>7.351861230225E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:77" x14ac:dyDescent="0.35">
       <c r="A11" s="6" t="s">
         <v>22</v>
       </c>
@@ -9403,7 +9403,7 @@
         <v>-5.174931031241E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:77" x14ac:dyDescent="0.35">
       <c r="A12" s="6" t="s">
         <v>23</v>
       </c>
@@ -9438,7 +9438,7 @@
         <v>-0.28626943427969997</v>
       </c>
     </row>
-    <row r="13" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:77" x14ac:dyDescent="0.35">
       <c r="A13" s="6" t="s">
         <v>24</v>
       </c>
@@ -9473,7 +9473,7 @@
         <v>0.19240811129338001</v>
       </c>
     </row>
-    <row r="14" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:77" x14ac:dyDescent="0.35">
       <c r="A14" s="6" t="s">
         <v>25</v>
       </c>
@@ -9507,9 +9507,38 @@
       <c r="K14" s="1">
         <v>0.27599205988476</v>
       </c>
-      <c r="Y14" s="2"/>
+      <c r="AB14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD14" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AF14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AG14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AH14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AI14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AJ14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AK14" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="15" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:77" x14ac:dyDescent="0.35">
       <c r="A15" s="6" t="s">
         <v>26</v>
       </c>
@@ -9543,8 +9572,51 @@
       <c r="K15" s="1">
         <v>1.0522149099460001E-2</v>
       </c>
+      <c r="AA15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB15" s="1">
+        <f>SUMPRODUCT($Z$2:$BY$2, $Z2:$BY2)</f>
+        <v>0.40074752713226119</v>
+      </c>
+      <c r="AC15" s="1">
+        <f>SUMPRODUCT($Z$3:$BY$3, $Z2:$BY2)</f>
+        <v>-0.12535266090198965</v>
+      </c>
+      <c r="AD15" s="1">
+        <f>SUMPRODUCT($Z$4:$BY$4, $Z2:$BY2)</f>
+        <v>6.81622825456855E-3</v>
+      </c>
+      <c r="AE15" s="1">
+        <f t="shared" ref="AE15:AK15" si="0">SUMPRODUCT($Z$3:$BY$3, $Z2:$BY2)</f>
+        <v>-0.12535266090198965</v>
+      </c>
+      <c r="AF15" s="1">
+        <f t="shared" ref="AF15:AK15" si="1">SUMPRODUCT($Z$2:$BY$2, $Z2:$BY2)</f>
+        <v>0.40074752713226119</v>
+      </c>
+      <c r="AG15" s="1">
+        <f t="shared" ref="AG15:AK15" si="2">SUMPRODUCT($Z$3:$BY$3, $Z2:$BY2)</f>
+        <v>-0.12535266090198965</v>
+      </c>
+      <c r="AH15" s="1">
+        <f t="shared" ref="AH15:AK15" si="3">SUMPRODUCT($Z$2:$BY$2, $Z2:$BY2)</f>
+        <v>0.40074752713226119</v>
+      </c>
+      <c r="AI15" s="1">
+        <f t="shared" ref="AI15:AK15" si="4">SUMPRODUCT($Z$3:$BY$3, $Z2:$BY2)</f>
+        <v>-0.12535266090198965</v>
+      </c>
+      <c r="AJ15" s="1">
+        <f t="shared" ref="AJ15:AK15" si="5">SUMPRODUCT($Z$2:$BY$2, $Z2:$BY2)</f>
+        <v>0.40074752713226119</v>
+      </c>
+      <c r="AK15" s="1">
+        <f t="shared" ref="AK15" si="6">SUMPRODUCT($Z$3:$BY$3, $Z2:$BY2)</f>
+        <v>-0.12535266090198965</v>
+      </c>
     </row>
-    <row r="16" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:77" x14ac:dyDescent="0.35">
       <c r="A16" s="6" t="s">
         <v>27</v>
       </c>
@@ -9578,8 +9650,51 @@
       <c r="K16" s="1">
         <v>-9.467565310803E-2</v>
       </c>
+      <c r="AA16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB16" s="1">
+        <f t="shared" ref="AB16:AJ24" si="7">SUMPRODUCT($Z$2:$BY$2, $Z3:$BY3)</f>
+        <v>-0.12535266090198965</v>
+      </c>
+      <c r="AC16" s="1">
+        <f t="shared" ref="AC16:AK24" si="8">SUMPRODUCT($Z$3:$BY$3, $Z3:$BY3)</f>
+        <v>0.51745018498646977</v>
+      </c>
+      <c r="AD16" s="1">
+        <f t="shared" ref="AD16:AD24" si="9">SUMPRODUCT($Z$4:$BY$4, $Z3:$BY3)</f>
+        <v>5.6782368729381215E-2</v>
+      </c>
+      <c r="AE16" s="1">
+        <f t="shared" si="8"/>
+        <v>0.51745018498646977</v>
+      </c>
+      <c r="AF16" s="1">
+        <f t="shared" si="7"/>
+        <v>-0.12535266090198965</v>
+      </c>
+      <c r="AG16" s="1">
+        <f t="shared" si="8"/>
+        <v>0.51745018498646977</v>
+      </c>
+      <c r="AH16" s="1">
+        <f t="shared" si="7"/>
+        <v>-0.12535266090198965</v>
+      </c>
+      <c r="AI16" s="1">
+        <f t="shared" si="8"/>
+        <v>0.51745018498646977</v>
+      </c>
+      <c r="AJ16" s="1">
+        <f t="shared" si="7"/>
+        <v>-0.12535266090198965</v>
+      </c>
+      <c r="AK16" s="1">
+        <f t="shared" si="8"/>
+        <v>0.51745018498646977</v>
+      </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>28</v>
       </c>
@@ -9613,8 +9728,51 @@
       <c r="K17" s="1">
         <v>2.0530069272969999E-2</v>
       </c>
+      <c r="AA17" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB17" s="1">
+        <f t="shared" si="7"/>
+        <v>6.81622825456855E-3</v>
+      </c>
+      <c r="AC17" s="1">
+        <f t="shared" si="8"/>
+        <v>5.6782368729381215E-2</v>
+      </c>
+      <c r="AD17" s="1">
+        <f t="shared" si="9"/>
+        <v>0.45649423430762998</v>
+      </c>
+      <c r="AE17" s="1">
+        <f t="shared" si="8"/>
+        <v>5.6782368729381215E-2</v>
+      </c>
+      <c r="AF17" s="1">
+        <f t="shared" si="7"/>
+        <v>6.81622825456855E-3</v>
+      </c>
+      <c r="AG17" s="1">
+        <f t="shared" si="8"/>
+        <v>5.6782368729381215E-2</v>
+      </c>
+      <c r="AH17" s="1">
+        <f t="shared" si="7"/>
+        <v>6.81622825456855E-3</v>
+      </c>
+      <c r="AI17" s="1">
+        <f t="shared" si="8"/>
+        <v>5.6782368729381215E-2</v>
+      </c>
+      <c r="AJ17" s="1">
+        <f t="shared" si="7"/>
+        <v>6.81622825456855E-3</v>
+      </c>
+      <c r="AK17" s="1">
+        <f t="shared" si="8"/>
+        <v>5.6782368729381215E-2</v>
+      </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>29</v>
       </c>
@@ -9648,8 +9806,51 @@
       <c r="K18" s="1">
         <v>0.14993945639133999</v>
       </c>
+      <c r="AA18" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB18" s="1">
+        <f t="shared" si="7"/>
+        <v>-8.4201125825136627E-2</v>
+      </c>
+      <c r="AC18" s="1">
+        <f t="shared" si="8"/>
+        <v>-2.2594722860546992E-2</v>
+      </c>
+      <c r="AD18" s="1">
+        <f t="shared" si="9"/>
+        <v>4.1909981631623565E-2</v>
+      </c>
+      <c r="AE18" s="1">
+        <f t="shared" si="8"/>
+        <v>-2.2594722860546992E-2</v>
+      </c>
+      <c r="AF18" s="1">
+        <f t="shared" si="7"/>
+        <v>-8.4201125825136627E-2</v>
+      </c>
+      <c r="AG18" s="1">
+        <f t="shared" si="8"/>
+        <v>-2.2594722860546992E-2</v>
+      </c>
+      <c r="AH18" s="1">
+        <f t="shared" si="7"/>
+        <v>-8.4201125825136627E-2</v>
+      </c>
+      <c r="AI18" s="1">
+        <f t="shared" si="8"/>
+        <v>-2.2594722860546992E-2</v>
+      </c>
+      <c r="AJ18" s="1">
+        <f t="shared" si="7"/>
+        <v>-8.4201125825136627E-2</v>
+      </c>
+      <c r="AK18" s="1">
+        <f t="shared" si="8"/>
+        <v>-2.2594722860546992E-2</v>
+      </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>30</v>
       </c>
@@ -9683,8 +9884,51 @@
       <c r="K19" s="1">
         <v>7.1456051653370004E-2</v>
       </c>
+      <c r="AA19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB19" s="1">
+        <f t="shared" si="7"/>
+        <v>5.3821559691754436E-2</v>
+      </c>
+      <c r="AC19" s="1">
+        <f t="shared" si="8"/>
+        <v>2.2986906484088916E-2</v>
+      </c>
+      <c r="AD19" s="1">
+        <f t="shared" si="9"/>
+        <v>-5.6803876383057436E-2</v>
+      </c>
+      <c r="AE19" s="1">
+        <f t="shared" si="8"/>
+        <v>2.2986906484088916E-2</v>
+      </c>
+      <c r="AF19" s="1">
+        <f t="shared" si="7"/>
+        <v>5.3821559691754436E-2</v>
+      </c>
+      <c r="AG19" s="1">
+        <f t="shared" si="8"/>
+        <v>2.2986906484088916E-2</v>
+      </c>
+      <c r="AH19" s="1">
+        <f t="shared" si="7"/>
+        <v>5.3821559691754436E-2</v>
+      </c>
+      <c r="AI19" s="1">
+        <f t="shared" si="8"/>
+        <v>2.2986906484088916E-2</v>
+      </c>
+      <c r="AJ19" s="1">
+        <f t="shared" si="7"/>
+        <v>5.3821559691754436E-2</v>
+      </c>
+      <c r="AK19" s="1">
+        <f t="shared" si="8"/>
+        <v>2.2986906484088916E-2</v>
+      </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>31</v>
       </c>
@@ -9718,8 +9962,51 @@
       <c r="K20" s="1">
         <v>7.49406617897E-3</v>
       </c>
+      <c r="AA20" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB20" s="1">
+        <f t="shared" si="7"/>
+        <v>1.8002171992056615E-2</v>
+      </c>
+      <c r="AC20" s="1">
+        <f t="shared" si="8"/>
+        <v>3.4497410906390538E-2</v>
+      </c>
+      <c r="AD20" s="1">
+        <f t="shared" si="9"/>
+        <v>-2.3737351470099846E-3</v>
+      </c>
+      <c r="AE20" s="1">
+        <f t="shared" si="8"/>
+        <v>3.4497410906390538E-2</v>
+      </c>
+      <c r="AF20" s="1">
+        <f t="shared" si="7"/>
+        <v>1.8002171992056615E-2</v>
+      </c>
+      <c r="AG20" s="1">
+        <f t="shared" si="8"/>
+        <v>3.4497410906390538E-2</v>
+      </c>
+      <c r="AH20" s="1">
+        <f t="shared" si="7"/>
+        <v>1.8002171992056615E-2</v>
+      </c>
+      <c r="AI20" s="1">
+        <f t="shared" si="8"/>
+        <v>3.4497410906390538E-2</v>
+      </c>
+      <c r="AJ20" s="1">
+        <f t="shared" si="7"/>
+        <v>1.8002171992056615E-2</v>
+      </c>
+      <c r="AK20" s="1">
+        <f t="shared" si="8"/>
+        <v>3.4497410906390538E-2</v>
+      </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>32</v>
       </c>
@@ -9753,8 +10040,51 @@
       <c r="K21" s="1">
         <v>0.24874907140051</v>
       </c>
+      <c r="AA21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AB21" s="1">
+        <f t="shared" si="7"/>
+        <v>-7.1270250078944988E-3</v>
+      </c>
+      <c r="AC21" s="1">
+        <f t="shared" si="8"/>
+        <v>2.3320864081260446E-2</v>
+      </c>
+      <c r="AD21" s="1">
+        <f>SUMPRODUCT($Z8:$BY8, $Z$4:$BY$4)</f>
+        <v>7.6273610553272836E-2</v>
+      </c>
+      <c r="AE21" s="1">
+        <f t="shared" si="8"/>
+        <v>2.3320864081260446E-2</v>
+      </c>
+      <c r="AF21" s="1">
+        <f t="shared" si="7"/>
+        <v>-7.1270250078944988E-3</v>
+      </c>
+      <c r="AG21" s="1">
+        <f t="shared" si="8"/>
+        <v>2.3320864081260446E-2</v>
+      </c>
+      <c r="AH21" s="1">
+        <f t="shared" si="7"/>
+        <v>-7.1270250078944988E-3</v>
+      </c>
+      <c r="AI21" s="1">
+        <f t="shared" si="8"/>
+        <v>2.3320864081260446E-2</v>
+      </c>
+      <c r="AJ21" s="1">
+        <f t="shared" si="7"/>
+        <v>-7.1270250078944988E-3</v>
+      </c>
+      <c r="AK21" s="1">
+        <f t="shared" si="8"/>
+        <v>2.3320864081260446E-2</v>
+      </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>33</v>
       </c>
@@ -9788,8 +10118,51 @@
       <c r="K22" s="1">
         <v>0.47059004220890999</v>
       </c>
+      <c r="AA22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB22" s="1">
+        <f t="shared" si="7"/>
+        <v>2.132281900661466E-2</v>
+      </c>
+      <c r="AC22" s="1">
+        <f t="shared" si="8"/>
+        <v>3.1109479176826573E-2</v>
+      </c>
+      <c r="AD22" s="1">
+        <f t="shared" si="9"/>
+        <v>5.4662215143406433E-2</v>
+      </c>
+      <c r="AE22" s="1">
+        <f t="shared" si="8"/>
+        <v>3.1109479176826573E-2</v>
+      </c>
+      <c r="AF22" s="1">
+        <f t="shared" si="7"/>
+        <v>2.132281900661466E-2</v>
+      </c>
+      <c r="AG22" s="1">
+        <f t="shared" si="8"/>
+        <v>3.1109479176826573E-2</v>
+      </c>
+      <c r="AH22" s="1">
+        <f t="shared" si="7"/>
+        <v>2.132281900661466E-2</v>
+      </c>
+      <c r="AI22" s="1">
+        <f t="shared" si="8"/>
+        <v>3.1109479176826573E-2</v>
+      </c>
+      <c r="AJ22" s="1">
+        <f t="shared" si="7"/>
+        <v>2.132281900661466E-2</v>
+      </c>
+      <c r="AK22" s="1">
+        <f t="shared" si="8"/>
+        <v>3.1109479176826573E-2</v>
+      </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>34</v>
       </c>
@@ -9823,8 +10196,51 @@
       <c r="K23" s="1">
         <v>-3.9232069048429997E-2</v>
       </c>
+      <c r="AA23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB23" s="1">
+        <f t="shared" si="7"/>
+        <v>-1.0634752812232392E-2</v>
+      </c>
+      <c r="AC23" s="1">
+        <f t="shared" si="8"/>
+        <v>-2.1205454231651107E-2</v>
+      </c>
+      <c r="AD23" s="1">
+        <f t="shared" si="9"/>
+        <v>-7.2358195204929318E-4</v>
+      </c>
+      <c r="AE23" s="1">
+        <f t="shared" si="8"/>
+        <v>-2.1205454231651107E-2</v>
+      </c>
+      <c r="AF23" s="1">
+        <f t="shared" si="7"/>
+        <v>-1.0634752812232392E-2</v>
+      </c>
+      <c r="AG23" s="1">
+        <f t="shared" si="8"/>
+        <v>-2.1205454231651107E-2</v>
+      </c>
+      <c r="AH23" s="1">
+        <f t="shared" si="7"/>
+        <v>-1.0634752812232392E-2</v>
+      </c>
+      <c r="AI23" s="1">
+        <f t="shared" si="8"/>
+        <v>-2.1205454231651107E-2</v>
+      </c>
+      <c r="AJ23" s="1">
+        <f t="shared" si="7"/>
+        <v>-1.0634752812232392E-2</v>
+      </c>
+      <c r="AK23" s="1">
+        <f t="shared" si="8"/>
+        <v>-2.1205454231651107E-2</v>
+      </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>35</v>
       </c>
@@ -9858,8 +10274,51 @@
       <c r="K24" s="1">
         <v>-4.4279889366E-4</v>
       </c>
+      <c r="AA24" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB24" s="1">
+        <f t="shared" si="7"/>
+        <v>1.1997430005586597E-2</v>
+      </c>
+      <c r="AC24" s="1">
+        <f t="shared" si="8"/>
+        <v>-3.6681786325762404E-2</v>
+      </c>
+      <c r="AD24" s="1">
+        <f t="shared" si="9"/>
+        <v>0.10837225157799839</v>
+      </c>
+      <c r="AE24" s="1">
+        <f t="shared" si="8"/>
+        <v>-3.6681786325762404E-2</v>
+      </c>
+      <c r="AF24" s="1">
+        <f t="shared" si="7"/>
+        <v>1.1997430005586597E-2</v>
+      </c>
+      <c r="AG24" s="1">
+        <f t="shared" si="8"/>
+        <v>-3.6681786325762404E-2</v>
+      </c>
+      <c r="AH24" s="1">
+        <f t="shared" si="7"/>
+        <v>1.1997430005586597E-2</v>
+      </c>
+      <c r="AI24" s="1">
+        <f t="shared" si="8"/>
+        <v>-3.6681786325762404E-2</v>
+      </c>
+      <c r="AJ24" s="1">
+        <f t="shared" si="7"/>
+        <v>1.1997430005586597E-2</v>
+      </c>
+      <c r="AK24" s="1">
+        <f>SUMPRODUCT($Z$3:$BY$3, $Z11:$BY11)</f>
+        <v>-3.6681786325762404E-2</v>
+      </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>36</v>
       </c>
@@ -9894,7 +10353,7 @@
         <v>-1.060552148391E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>37</v>
       </c>
@@ -9929,7 +10388,7 @@
         <v>-1.566147018024E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>38</v>
       </c>
@@ -9963,8 +10422,12 @@
       <c r="K27" s="1">
         <v>8.3797809050280003E-2</v>
       </c>
+      <c r="AB27" s="1">
+        <f>SUMPRODUCT(Z11:BY11, Z11:BY11)</f>
+        <v>0.54073457781268297</v>
+      </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>12</v>
       </c>
@@ -9999,12 +10462,12 @@
         <v>-0.11558729628427999</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:37" x14ac:dyDescent="0.35">
       <c r="B32" s="1" t="s">
         <v>0</v>
       </c>
@@ -10036,12 +10499,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B33" s="1">
-        <f t="array" ref="B33">SUMPRODUCT($B$2:$B$28,B$2:B$28)</f>
+        <f>SUMPRODUCT($B$2:$B$28,B$2:B$28)</f>
         <v>0.99999999999999778</v>
       </c>
       <c r="C33" s="1">
@@ -10053,35 +10516,35 @@
         <v>5.134781488891349E-16</v>
       </c>
       <c r="E33" s="1">
-        <f t="shared" ref="E33:K33" si="0">SUMPRODUCT($B$2:$B$28,E$2:E$28)</f>
+        <f t="shared" ref="E33:K33" si="10">SUMPRODUCT($B$2:$B$28,E$2:E$28)</f>
         <v>5.8564264548977008E-15</v>
       </c>
       <c r="F33" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="10"/>
         <v>2.5569824035898137E-15</v>
       </c>
       <c r="G33" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="10"/>
         <v>-3.2508717939805365E-15</v>
       </c>
       <c r="H33" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="10"/>
         <v>-4.1078251911130792E-15</v>
       </c>
       <c r="I33" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="10"/>
         <v>-3.6290415117434804E-15</v>
       </c>
       <c r="J33" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="10"/>
         <v>3.9889966330086679E-15</v>
       </c>
       <c r="K33" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="10"/>
         <v>3.1988300897012323E-15</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>1</v>
       </c>
@@ -10090,43 +10553,43 @@
         <v>-5.2388648974499574E-16</v>
       </c>
       <c r="C34" s="1">
-        <f t="shared" ref="C34:K34" si="1">SUMPRODUCT($C$2:$C$28,C$2:C$28)</f>
+        <f>SUMPRODUCT($C$2:$C$28,C$2:C$28)</f>
         <v>0.999999999999996</v>
       </c>
       <c r="D34" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="C34:K34" si="11">SUMPRODUCT($C$2:$C$28,D$2:D$28)</f>
         <v>6.7584826624056404E-15</v>
       </c>
       <c r="E34" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="11"/>
         <v>2.5656560209696977E-15</v>
       </c>
       <c r="F34" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="11"/>
         <v>-1.1796119636642288E-16</v>
       </c>
       <c r="G34" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="11"/>
         <v>-8.5868812060851951E-15</v>
       </c>
       <c r="H34" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="11"/>
         <v>-8.156669784042947E-15</v>
       </c>
       <c r="I34" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="11"/>
         <v>-6.0715321659188248E-16</v>
       </c>
       <c r="J34" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="11"/>
         <v>7.4757908197220502E-15</v>
       </c>
       <c r="K34" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="11"/>
         <v>5.8772431366094224E-15</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>2</v>
       </c>
@@ -10135,43 +10598,43 @@
         <v>5.134781488891349E-16</v>
       </c>
       <c r="C35" s="1">
-        <f t="shared" ref="C35:K35" si="2">SUMPRODUCT($D$2:$D$28,C$2:C$28)</f>
+        <f t="shared" ref="C35:K35" si="12">SUMPRODUCT($D$2:$D$28,C$2:C$28)</f>
         <v>6.7584826624056404E-15</v>
       </c>
       <c r="D35" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="12"/>
         <v>1.0000000000000091</v>
       </c>
       <c r="E35" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="12"/>
         <v>-1.6479873021779667E-15</v>
       </c>
       <c r="F35" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="12"/>
         <v>-5.4956039718945249E-15</v>
       </c>
       <c r="G35" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="12"/>
         <v>6.3143934525555778E-16</v>
       </c>
       <c r="H35" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="12"/>
         <v>6.2484739604684592E-15</v>
       </c>
       <c r="I35" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="12"/>
         <v>-5.5337678883660146E-15</v>
       </c>
       <c r="J35" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="12"/>
         <v>-2.5743296383495817E-15</v>
       </c>
       <c r="K35" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="12"/>
         <v>2.4528989950312052E-15</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>3</v>
       </c>
@@ -10180,43 +10643,43 @@
         <v>5.8564264548977008E-15</v>
       </c>
       <c r="C36" s="1">
-        <f t="shared" ref="C36:K36" si="3">SUMPRODUCT($E$2:$E$28,C$2:C$28)</f>
+        <f t="shared" ref="C36:K36" si="13">SUMPRODUCT($E$2:$E$28,C$2:C$28)</f>
         <v>2.5656560209696977E-15</v>
       </c>
       <c r="D36" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="13"/>
         <v>-1.6479873021779667E-15</v>
       </c>
       <c r="E36" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="13"/>
         <v>1.0000000000000022</v>
       </c>
       <c r="F36" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="13"/>
         <v>-5.4990734188464785E-15</v>
       </c>
       <c r="G36" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="13"/>
         <v>2.8102520310824275E-16</v>
       </c>
       <c r="H36" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="13"/>
         <v>-7.5755374195907166E-15</v>
       </c>
       <c r="I36" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="13"/>
         <v>-8.3127948968808596E-15</v>
       </c>
       <c r="J36" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="13"/>
         <v>2.9386215683047112E-15</v>
       </c>
       <c r="K36" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="13"/>
         <v>3.1225022567582528E-16</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>4</v>
       </c>
@@ -10225,31 +10688,31 @@
         <v>2.5569824035898137E-15</v>
       </c>
       <c r="C37" s="1">
-        <f t="shared" ref="C37:K37" si="4">SUMPRODUCT($F$2:$F$28,C$2:C$28)</f>
+        <f t="shared" ref="C37:K37" si="14">SUMPRODUCT($F$2:$F$28,C$2:C$28)</f>
         <v>-1.1796119636642288E-16</v>
       </c>
       <c r="D37" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>-5.4956039718945249E-15</v>
       </c>
       <c r="E37" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>-5.4990734188464785E-15</v>
       </c>
       <c r="F37" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>0.999999999999997</v>
       </c>
       <c r="G37" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>2.4286128663675299E-16</v>
       </c>
       <c r="H37" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>6.3560268159790212E-15</v>
       </c>
       <c r="I37" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>-5.3602955407683339E-15</v>
       </c>
       <c r="J37" s="1">
@@ -10257,11 +10720,11 @@
         <v>1.0683728207672161E-15</v>
       </c>
       <c r="K37" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>-9.1142371427821445E-15</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>5</v>
       </c>
@@ -10270,43 +10733,43 @@
         <v>-3.2508717939805365E-15</v>
       </c>
       <c r="C38" s="1">
-        <f t="shared" ref="C38:K38" si="5">SUMPRODUCT($G$2:$G$28,C$2:C$28)</f>
+        <f t="shared" ref="C38:K38" si="15">SUMPRODUCT($G$2:$G$28,C$2:C$28)</f>
         <v>-8.5868812060851951E-15</v>
       </c>
       <c r="D38" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="15"/>
         <v>6.3143934525555778E-16</v>
       </c>
       <c r="E38" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="15"/>
         <v>2.8102520310824275E-16</v>
       </c>
       <c r="F38" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="15"/>
         <v>2.4286128663675299E-16</v>
       </c>
       <c r="G38" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="15"/>
         <v>1.0000000000000098</v>
       </c>
       <c r="H38" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="15"/>
         <v>-2.1389140458794031E-15</v>
       </c>
       <c r="I38" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="15"/>
         <v>4.2847669856627135E-16</v>
       </c>
       <c r="J38" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="15"/>
         <v>1.8726339923169633E-15</v>
       </c>
       <c r="K38" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="15"/>
         <v>8.7430063189231078E-16</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>6</v>
       </c>
@@ -10315,43 +10778,43 @@
         <v>-4.1078251911130792E-15</v>
       </c>
       <c r="C39" s="1">
-        <f t="shared" ref="C39:K39" si="6">SUMPRODUCT($H$2:$H$28,C$2:C$28)</f>
+        <f t="shared" ref="C39:K39" si="16">SUMPRODUCT($H$2:$H$28,C$2:C$28)</f>
         <v>-8.156669784042947E-15</v>
       </c>
       <c r="D39" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="16"/>
         <v>6.2484739604684592E-15</v>
       </c>
       <c r="E39" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="16"/>
         <v>-7.5755374195907166E-15</v>
       </c>
       <c r="F39" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="16"/>
         <v>6.3560268159790212E-15</v>
       </c>
       <c r="G39" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="16"/>
         <v>-2.1389140458794031E-15</v>
       </c>
       <c r="H39" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="16"/>
         <v>1.0000000000000089</v>
       </c>
       <c r="I39" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="16"/>
         <v>7.8929918156944723E-16</v>
       </c>
       <c r="J39" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="16"/>
         <v>-5.2978454956331689E-15</v>
       </c>
       <c r="K39" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="16"/>
         <v>1.1568870861289327E-14</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>7</v>
       </c>
@@ -10360,43 +10823,43 @@
         <v>-3.6290415117434804E-15</v>
       </c>
       <c r="C40" s="1">
-        <f t="shared" ref="C40:K40" si="7">SUMPRODUCT($I$2:$I$28,C$2:C$28)</f>
+        <f t="shared" ref="C40:K40" si="17">SUMPRODUCT($I$2:$I$28,C$2:C$28)</f>
         <v>-6.0715321659188248E-16</v>
       </c>
       <c r="D40" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="17"/>
         <v>-5.5337678883660146E-15</v>
       </c>
       <c r="E40" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="17"/>
         <v>-8.3127948968808596E-15</v>
       </c>
       <c r="F40" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="17"/>
         <v>-5.3602955407683339E-15</v>
       </c>
       <c r="G40" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="17"/>
         <v>4.2847669856627135E-16</v>
       </c>
       <c r="H40" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="17"/>
         <v>7.8929918156944723E-16</v>
       </c>
       <c r="I40" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="17"/>
         <v>0.99999999999999944</v>
       </c>
       <c r="J40" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="17"/>
         <v>1.7329887525008303E-15</v>
       </c>
       <c r="K40" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="17"/>
         <v>-3.3601593729670753E-15</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>8</v>
       </c>
@@ -10405,43 +10868,43 @@
         <v>3.9889966330086679E-15</v>
       </c>
       <c r="C41" s="1">
-        <f t="shared" ref="C41:K41" si="8">SUMPRODUCT($J$2:$J$28,C$2:C$28)</f>
+        <f t="shared" ref="C41:K41" si="18">SUMPRODUCT($J$2:$J$28,C$2:C$28)</f>
         <v>7.4757908197220502E-15</v>
       </c>
       <c r="D41" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="18"/>
         <v>-2.5743296383495817E-15</v>
       </c>
       <c r="E41" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="18"/>
         <v>2.9386215683047112E-15</v>
       </c>
       <c r="F41" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="18"/>
         <v>1.0683728207672161E-15</v>
       </c>
       <c r="G41" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="18"/>
         <v>1.8726339923169633E-15</v>
       </c>
       <c r="H41" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="18"/>
         <v>-5.2978454956331689E-15</v>
       </c>
       <c r="I41" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="18"/>
         <v>1.7329887525008303E-15</v>
       </c>
       <c r="J41" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="18"/>
         <v>0.99999999999999201</v>
       </c>
       <c r="K41" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="18"/>
         <v>1.9372524417970993E-15</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>9</v>
       </c>
@@ -10450,40 +10913,46 @@
         <v>3.1988300897012323E-15</v>
       </c>
       <c r="C42" s="1">
-        <f t="shared" ref="C42:K42" si="9">SUMPRODUCT($K$2:$K$28,C$2:C$28)</f>
+        <f t="shared" ref="C42:K42" si="19">SUMPRODUCT($K$2:$K$28,C$2:C$28)</f>
         <v>5.8772431366094224E-15</v>
       </c>
       <c r="D42" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="19"/>
         <v>2.4528989950312052E-15</v>
       </c>
       <c r="E42" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="19"/>
         <v>3.1225022567582528E-16</v>
       </c>
       <c r="F42" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="19"/>
         <v>-9.1142371427821445E-15</v>
       </c>
       <c r="G42" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="19"/>
         <v>8.7430063189231078E-16</v>
       </c>
       <c r="H42" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="19"/>
         <v>1.1568870861289327E-14</v>
       </c>
       <c r="I42" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="19"/>
         <v>-3.3601593729670753E-15</v>
       </c>
       <c r="J42" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="19"/>
         <v>1.9372524417970993E-15</v>
       </c>
       <c r="K42" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="19"/>
         <v>1.0000000000000029</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B51" s="1">
+        <f>SUMPRODUCT(B2:B28,B2:B28)</f>
+        <v>0.99999999999999778</v>
       </c>
     </row>
   </sheetData>
@@ -10496,17 +10965,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BY47"/>
   <sheetViews>
-    <sheetView topLeftCell="S1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H5" sqref="A5:XFD5"/>
+    <sheetView topLeftCell="L1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.42578125" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="15.44140625" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="30.140625" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="15.42578125" style="1"/>
+    <col min="1" max="1" width="30.109375" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="15.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:77" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -10514,7 +10983,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:77" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -10738,7 +11207,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:77" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>13</v>
       </c>
@@ -10968,7 +11437,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:77" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
         <v>14</v>
       </c>
@@ -11198,7 +11667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:77" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
         <v>15</v>
       </c>
@@ -11428,7 +11897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:77" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
         <v>16</v>
       </c>
@@ -11658,7 +12127,7 @@
         <v>0.22920641104118</v>
       </c>
     </row>
-    <row r="7" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:77" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
         <v>17</v>
       </c>
@@ -11888,7 +12357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:77" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
         <v>18</v>
       </c>
@@ -12118,7 +12587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:77" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="s">
         <v>19</v>
       </c>
@@ -12348,7 +12817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:77" x14ac:dyDescent="0.35">
       <c r="A10" s="6" t="s">
         <v>20</v>
       </c>
@@ -12578,7 +13047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:77" x14ac:dyDescent="0.35">
       <c r="A11" s="6" t="s">
         <v>21</v>
       </c>
@@ -12808,7 +13277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:77" x14ac:dyDescent="0.35">
       <c r="A12" s="6" t="s">
         <v>22</v>
       </c>
@@ -13038,7 +13507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:77" x14ac:dyDescent="0.35">
       <c r="A13" s="6" t="s">
         <v>23</v>
       </c>
@@ -13073,7 +13542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:77" x14ac:dyDescent="0.35">
       <c r="A14" s="6" t="s">
         <v>24</v>
       </c>
@@ -13108,7 +13577,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:77" x14ac:dyDescent="0.35">
       <c r="A15" s="6" t="s">
         <v>25</v>
       </c>
@@ -13143,7 +13612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:77" x14ac:dyDescent="0.35">
       <c r="A16" s="6" t="s">
         <v>26</v>
       </c>
@@ -13178,7 +13647,7 @@
         <v>2.4849899980329999E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:77" x14ac:dyDescent="0.35">
       <c r="A17" s="6" t="s">
         <v>27</v>
       </c>
@@ -13214,7 +13683,7 @@
       </c>
       <c r="N17" s="2"/>
     </row>
-    <row r="18" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:77" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>28</v>
       </c>
@@ -13249,7 +13718,7 @@
         <v>1.204106142061E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:77" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>29</v>
       </c>
@@ -13287,7 +13756,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="20" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:77" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>30</v>
       </c>
@@ -13322,7 +13791,7 @@
         <v>1.602828159374E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:77" ht="37.5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:77" ht="36" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>31</v>
       </c>
@@ -13616,7 +14085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:77" ht="56.25" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:77" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>32</v>
       </c>
@@ -13910,7 +14379,7 @@
         <v>4.9470455246544117E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:77" ht="56.25" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:77" ht="54" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>33</v>
       </c>
@@ -14204,7 +14673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:77" ht="56.25" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:77" ht="54" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>34</v>
       </c>
@@ -14498,7 +14967,7 @@
         <v>6.1890449802418108E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:77" ht="56.25" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:77" ht="54" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>35</v>
       </c>
@@ -14792,7 +15261,7 @@
         <v>0.17600041319187054</v>
       </c>
     </row>
-    <row r="26" spans="1:77" ht="56.25" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:77" ht="54" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>36</v>
       </c>
@@ -15086,7 +15555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:77" ht="56.25" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:77" ht="54" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>37</v>
       </c>
@@ -15380,7 +15849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:77" ht="56.25" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:77" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>38</v>
       </c>
@@ -15674,7 +16143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:77" ht="56.25" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:77" ht="54" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>12</v>
       </c>
@@ -15968,7 +16437,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:77" x14ac:dyDescent="0.35">
       <c r="M30" s="6" t="s">
         <v>22</v>
       </c>
@@ -16229,7 +16698,7 @@
         <v>3.08778469961489E-5</v>
       </c>
     </row>
-    <row r="31" spans="1:77" ht="56.25" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:77" ht="54" x14ac:dyDescent="0.35">
       <c r="M31" s="6" t="s">
         <v>23</v>
       </c>
@@ -16490,7 +16959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:77" ht="56.25" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:77" ht="54" x14ac:dyDescent="0.35">
       <c r="M32" s="6" t="s">
         <v>24</v>
       </c>
@@ -16751,7 +17220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="13:77" ht="56.25" x14ac:dyDescent="0.3">
+    <row r="33" spans="13:77" ht="54" x14ac:dyDescent="0.35">
       <c r="M33" s="6" t="s">
         <v>25</v>
       </c>
@@ -17012,7 +17481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="13:77" ht="56.25" x14ac:dyDescent="0.3">
+    <row r="34" spans="13:77" ht="54" x14ac:dyDescent="0.35">
       <c r="M34" s="6" t="s">
         <v>26</v>
       </c>
@@ -17273,7 +17742,7 @@
         <v>4.4361574415888519E-3</v>
       </c>
     </row>
-    <row r="35" spans="13:77" ht="56.25" x14ac:dyDescent="0.3">
+    <row r="35" spans="13:77" ht="54" x14ac:dyDescent="0.35">
       <c r="M35" s="6" t="s">
         <v>27</v>
       </c>
@@ -17534,7 +18003,7 @@
         <v>3.8615616041242815E-4</v>
       </c>
     </row>
-    <row r="36" spans="13:77" x14ac:dyDescent="0.3">
+    <row r="36" spans="13:77" x14ac:dyDescent="0.35">
       <c r="M36" s="1" t="s">
         <v>28</v>
       </c>
@@ -17795,7 +18264,7 @@
         <v>2.4811240745908499E-3</v>
       </c>
     </row>
-    <row r="37" spans="13:77" x14ac:dyDescent="0.3">
+    <row r="37" spans="13:77" x14ac:dyDescent="0.35">
       <c r="M37" s="1" t="s">
         <v>29</v>
       </c>
@@ -18056,7 +18525,7 @@
         <v>1.696696193434156E-3</v>
       </c>
     </row>
-    <row r="38" spans="13:77" x14ac:dyDescent="0.3">
+    <row r="38" spans="13:77" x14ac:dyDescent="0.35">
       <c r="M38" s="1" t="s">
         <v>30</v>
       </c>
@@ -18317,7 +18786,7 @@
         <v>1.5163114110870277E-3</v>
       </c>
     </row>
-    <row r="39" spans="13:77" x14ac:dyDescent="0.3">
+    <row r="39" spans="13:77" x14ac:dyDescent="0.35">
       <c r="M39" s="1" t="s">
         <v>31</v>
       </c>
@@ -18578,7 +19047,7 @@
         <v>8.092659432018345E-3</v>
       </c>
     </row>
-    <row r="40" spans="13:77" x14ac:dyDescent="0.3">
+    <row r="40" spans="13:77" x14ac:dyDescent="0.35">
       <c r="M40" s="1" t="s">
         <v>32</v>
       </c>
@@ -18839,7 +19308,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="13:77" x14ac:dyDescent="0.3">
+    <row r="41" spans="13:77" x14ac:dyDescent="0.35">
       <c r="M41" s="1" t="s">
         <v>33</v>
       </c>
@@ -19100,7 +19569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="13:77" x14ac:dyDescent="0.3">
+    <row r="42" spans="13:77" x14ac:dyDescent="0.35">
       <c r="M42" s="1" t="s">
         <v>34</v>
       </c>
@@ -19361,7 +19830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="13:77" x14ac:dyDescent="0.3">
+    <row r="43" spans="13:77" x14ac:dyDescent="0.35">
       <c r="M43" s="1" t="s">
         <v>35</v>
       </c>
@@ -19622,7 +20091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="13:77" x14ac:dyDescent="0.3">
+    <row r="44" spans="13:77" x14ac:dyDescent="0.35">
       <c r="M44" s="1" t="s">
         <v>36</v>
       </c>
@@ -19883,7 +20352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="13:77" x14ac:dyDescent="0.3">
+    <row r="45" spans="13:77" x14ac:dyDescent="0.35">
       <c r="M45" s="1" t="s">
         <v>37</v>
       </c>
@@ -20144,7 +20613,7 @@
         <v>6.4068606719233151E-3</v>
       </c>
     </row>
-    <row r="46" spans="13:77" x14ac:dyDescent="0.3">
+    <row r="46" spans="13:77" x14ac:dyDescent="0.35">
       <c r="M46" s="1" t="s">
         <v>38</v>
       </c>
@@ -20405,7 +20874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="13:77" x14ac:dyDescent="0.3">
+    <row r="47" spans="13:77" x14ac:dyDescent="0.35">
       <c r="M47" s="1" t="s">
         <v>12</v>
       </c>
@@ -20680,12 +21149,12 @@
       <selection activeCell="A2" sqref="A2:A28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.5703125" customWidth="1"/>
+    <col min="1" max="1" width="29.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:53" x14ac:dyDescent="0.3">
       <c r="B1" s="9" t="s">
         <v>40</v>
       </c>
@@ -20843,7 +21312,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="2" spans="1:53" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:53" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
@@ -21004,7 +21473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:53" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:53" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>14</v>
       </c>
@@ -21165,7 +21634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:53" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:53" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>15</v>
       </c>
@@ -21326,7 +21795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:53" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:53" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>16</v>
       </c>
@@ -21487,7 +21956,7 @@
         <v>0.25136562999363998</v>
       </c>
     </row>
-    <row r="6" spans="1:53" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:53" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>17</v>
       </c>
@@ -21648,7 +22117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:53" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:53" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>18</v>
       </c>
@@ -21809,7 +22278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:53" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:53" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>19</v>
       </c>
@@ -21970,7 +22439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:53" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:53" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>20</v>
       </c>
@@ -22131,7 +22600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:53" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:53" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>21</v>
       </c>
@@ -22292,7 +22761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:53" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:53" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>22</v>
       </c>
@@ -22453,7 +22922,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:53" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:53" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>23</v>
       </c>
@@ -22614,7 +23083,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:53" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:53" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>24</v>
       </c>
@@ -22775,7 +23244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:53" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:53" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>25</v>
       </c>
@@ -22936,7 +23405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:53" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:53" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>26</v>
       </c>
@@ -23097,7 +23566,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:53" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:53" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>27</v>
       </c>
@@ -23258,7 +23727,7 @@
         <v>0.31325220022476002</v>
       </c>
     </row>
-    <row r="17" spans="1:53" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:53" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>28</v>
       </c>
@@ -23419,7 +23888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:53" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:53" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>29</v>
       </c>
@@ -23580,7 +24049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:53" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:53" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>30</v>
       </c>
@@ -23741,7 +24210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:53" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:53" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
         <v>31</v>
       </c>
@@ -23902,7 +24371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:53" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:53" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
         <v>32</v>
       </c>
@@ -24063,7 +24532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:53" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:53" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
         <v>33</v>
       </c>
@@ -24224,7 +24693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:53" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:53" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
         <v>34</v>
       </c>
@@ -24385,7 +24854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:53" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:53" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
         <v>35</v>
       </c>
@@ -24546,7 +25015,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:53" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:53" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
         <v>36</v>
       </c>
@@ -24707,7 +25176,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:53" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:53" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
         <v>37</v>
       </c>
@@ -24868,7 +25337,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:53" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:53" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
         <v>38</v>
       </c>
@@ -25029,7 +25498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:53" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:53" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="7" t="s">
         <v>12</v>
       </c>
@@ -25199,18 +25668,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -25228,7 +25697,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>3</v>
       </c>
@@ -25246,7 +25715,7 @@
         <v>-13</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -25264,7 +25733,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -25279,7 +25748,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>1</v>
       </c>
@@ -25304,7 +25773,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>3</v>
       </c>
@@ -25329,7 +25798,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2</v>
       </c>
@@ -25354,7 +25823,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>4</v>
       </c>

</xml_diff>